<commit_message>
Using doc2vec to cluster albums.
</commit_message>
<xml_diff>
--- a/music_meta/ListeningLog.xlsx
+++ b/music_meta/ListeningLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\projects\castle_analysis\music_meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4D25F3-FE02-48F8-AAD1-8555D9042049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937BE043-3D24-4A79-9E26-250CE5FCFA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Artist</t>
   </si>
@@ -33,15 +33,9 @@
     <t>Date</t>
   </si>
   <si>
-    <t>SessionSource</t>
-  </si>
-  <si>
     <t>Flying Lotus</t>
   </si>
   <si>
-    <t>ReccomendationSource</t>
-  </si>
-  <si>
     <t>Album similarity to King Gizzar and the Lizard Wizard - Flying Microtonal Banana</t>
   </si>
   <si>
@@ -54,7 +48,85 @@
     <t>Initial Rating</t>
   </si>
   <si>
-    <t>After 3 songs I am really enjoying the artist so far and want to continue listening.</t>
+    <t>Alice Glass</t>
+  </si>
+  <si>
+    <t>Artist similarity to Crystal Castles</t>
+  </si>
+  <si>
+    <t>Arkaea</t>
+  </si>
+  <si>
+    <t>You Tube</t>
+  </si>
+  <si>
+    <t>Close match to artest embedding means for 'The Cure', 'Animals as Leaders', 'System of a Down'</t>
+  </si>
+  <si>
+    <t>Gorgon City</t>
+  </si>
+  <si>
+    <t>Sample from artist cluster (23): [Electronic, Drum and bass, Trance, EDM, House]</t>
+  </si>
+  <si>
+    <t>Easy to listen to, but a bit boring.</t>
+  </si>
+  <si>
+    <t>Pura Fé</t>
+  </si>
+  <si>
+    <t>Sample from artist cluster (58): [Jazz, Gypsy punk, Pop, Rock, Electric blues, …</t>
+  </si>
+  <si>
+    <t>Reccomendation Source</t>
+  </si>
+  <si>
+    <t>Session Source</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>The Gathering</t>
+  </si>
+  <si>
+    <t>Sample from artist cluster (80): [Symphonic metal, Progressive rock, Symphonic …</t>
+  </si>
+  <si>
+    <t>It seems listenable, but makes me want to hear the deftones instead.</t>
+  </si>
+  <si>
+    <t>I really like this artist so far. The sounds were pretty jazzy. A few of the songs had guest artists, which included Kendrick Lamar and Anderson Paak, both of whom I enjoy.</t>
+  </si>
+  <si>
+    <t>I really like them so far. It reminds me a bit of night wish, but with a bit softer or ambient sound. There were some sections of songs that came in very different from most of the songs sound, which was nice. The songs feel like they have a musical story/arc. The current song I am on "Heroes for Ghosts" has a horn part - awesome!</t>
+  </si>
+  <si>
+    <t>Was a former member of Crystal Castles. Generally interesting sounding, but the singers sounded a bit odd to me. I don't remember that voice grating me in Crystal Castles. I think it was similar, but it could be that the songs I listed to didn't break up the singing as much with other parts?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The first few songs are pretty interesting. It is different from what I typically listen to. The sounds are folky. It looks like a native American band. </t>
+  </si>
+  <si>
+    <t>Max Richter</t>
+  </si>
+  <si>
+    <t>Amazon Best of</t>
+  </si>
+  <si>
+    <t>Sample from artist cluster (17): [Electronic, Ambient, Art rock, Chamber jazz, …</t>
+  </si>
+  <si>
+    <t>Melanie Safka</t>
+  </si>
+  <si>
+    <t>Sample from artist cluster (7): [Alternative rock, Trip hop, post-industrial, …</t>
+  </si>
+  <si>
+    <t>I like the music, but it is something I would want to listen to when going to sleep or concentraing on something else.</t>
+  </si>
+  <si>
+    <t>I didn't expect her sound based on the top tagged genres. I like the songs so far. I recognized some of the songs by her and some sounded like covers. The sound seems more 70's folk style.</t>
   </si>
 </sst>
 </file>
@@ -90,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -99,6 +171,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -381,22 +456,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.26953125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="38.7265625" style="2" customWidth="1"/>
     <col min="6" max="6" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,36 +480,200 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="92" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="92" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="3">
         <v>44134</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1">
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4">
+        <v>44500</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44500</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44500</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44500</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="116" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44500</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1">
         <v>8</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44500</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44500</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>